<commit_message>
Update master_trail_income.xlsx for 2025-04
</commit_message>
<xml_diff>
--- a/app/trail-data/master_trail_income.xlsx
+++ b/app/trail-data/master_trail_income.xlsx
@@ -1,61 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\incentive-calculator\app\trail-data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13820" windowHeight="6890"/>
-  </bookViews>
   <sheets>
     <sheet name="TrailIncome" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Trail Income</t>
-  </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>HARSHAD NAGTILAK</t>
-  </si>
-  <si>
-    <t>HRUTWIK GARDI</t>
-  </si>
-  <si>
-    <t>PRATIK RAUL</t>
-  </si>
-  <si>
-    <t>PRATIK SHIRBHATE</t>
-  </si>
-  <si>
-    <t>SARANG THAKREY</t>
-  </si>
-  <si>
-    <t>SHUBHAM MUNDADA</t>
-  </si>
-  <si>
-    <t>YUKTA SONIGRA</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -92,14 +72,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -424,86 +396,159 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Trail Income</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Month</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>HARSHAD NAGTILAK</v>
       </c>
       <c r="B2">
-        <v>17833.768199999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>4</v>
+        <v>17833.7682</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>HRUTWIK GARDI</v>
       </c>
       <c r="B3">
         <v>463.1626</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>5</v>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>PRATIK RAUL</v>
       </c>
       <c r="B4">
         <v>18291.220999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>6</v>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>PRATIK SHIRBHATE</v>
       </c>
       <c r="B5">
-        <v>3813.1927999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>7</v>
+        <v>3813.1928</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>SARANG THAKREY</v>
       </c>
       <c r="B6">
-        <v>458.57619999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>8</v>
+        <v>458.5762</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>SHUBHAM MUNDADA</v>
       </c>
       <c r="B7">
-        <v>74462.300199999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>9</v>
+        <v>74462.3002</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>YUKTA SONIGRA</v>
       </c>
       <c r="B8">
-        <v>12699.603499999999</v>
+        <v>12699.6035</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>HARSHAD NAGTILAK</v>
+      </c>
+      <c r="B9">
+        <v>22913.3785</v>
+      </c>
+      <c r="C9" t="str">
+        <v>2025-04</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>HRUTWIK GARDI</v>
+      </c>
+      <c r="B10">
+        <v>592.861</v>
+      </c>
+      <c r="C10" t="str">
+        <v>2025-04</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>PRATIK RAUL</v>
+      </c>
+      <c r="B11">
+        <v>29943.4216</v>
+      </c>
+      <c r="C11" t="str">
+        <v>2025-04</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>PRATIK SHIRBHATE</v>
+      </c>
+      <c r="B12">
+        <v>1752.8626499999998</v>
+      </c>
+      <c r="C12" t="str">
+        <v>2025-04</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>SARANG THAKREY</v>
+      </c>
+      <c r="B13">
+        <v>557.0264</v>
+      </c>
+      <c r="C13" t="str">
+        <v>2025-04</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>SHUBHAM MUNDADA</v>
+      </c>
+      <c r="B14">
+        <v>89968.73989999996</v>
+      </c>
+      <c r="C14" t="str">
+        <v>2025-04</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>YUKTA SONIGRA</v>
+      </c>
+      <c r="B15">
+        <v>16846.567150000003</v>
+      </c>
+      <c r="C15" t="str">
+        <v>2025-04</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C8" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C15"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>